<commit_message>
Reorg and added related files
</commit_message>
<xml_diff>
--- a/TONS.xlsx
+++ b/TONS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="23420" windowHeight="16160" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="26720" windowHeight="16160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="142">
   <si>
     <t>60m00s</t>
   </si>
@@ -199,6 +199,252 @@
   </si>
   <si>
     <t>Transmissions</t>
+  </si>
+  <si>
+    <t>13m34s</t>
+  </si>
+  <si>
+    <t>14m19s</t>
+  </si>
+  <si>
+    <t>17m31s</t>
+  </si>
+  <si>
+    <t>21m01s</t>
+  </si>
+  <si>
+    <t>23m00s</t>
+  </si>
+  <si>
+    <t>24m56s</t>
+  </si>
+  <si>
+    <t>27m55s</t>
+  </si>
+  <si>
+    <t>29m51s</t>
+  </si>
+  <si>
+    <t>32m51s</t>
+  </si>
+  <si>
+    <t>35m35s</t>
+  </si>
+  <si>
+    <t>40m55s</t>
+  </si>
+  <si>
+    <t>45m05s</t>
+  </si>
+  <si>
+    <t>50m28s</t>
+  </si>
+  <si>
+    <t>54m38s</t>
+  </si>
+  <si>
+    <t>62m00s</t>
+  </si>
+  <si>
+    <t>13m00s</t>
+  </si>
+  <si>
+    <t>13m22s</t>
+  </si>
+  <si>
+    <t>14m25s</t>
+  </si>
+  <si>
+    <t>01h01m</t>
+  </si>
+  <si>
+    <t>15m50s</t>
+  </si>
+  <si>
+    <t>17m27s</t>
+  </si>
+  <si>
+    <t>19m01s</t>
+  </si>
+  <si>
+    <t>20m52s</t>
+  </si>
+  <si>
+    <t>22m48s</t>
+  </si>
+  <si>
+    <t>25m28s</t>
+  </si>
+  <si>
+    <t>28m11s</t>
+  </si>
+  <si>
+    <t>30m05s</t>
+  </si>
+  <si>
+    <t>33m35s</t>
+  </si>
+  <si>
+    <t>37m15s</t>
+  </si>
+  <si>
+    <t>40m33s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46m41s </t>
+  </si>
+  <si>
+    <t>50m01s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55m46s </t>
+  </si>
+  <si>
+    <t>12m59s</t>
+  </si>
+  <si>
+    <t>13m20s</t>
+  </si>
+  <si>
+    <t>14m32s</t>
+  </si>
+  <si>
+    <t>17m19s</t>
+  </si>
+  <si>
+    <t>19m13s</t>
+  </si>
+  <si>
+    <t>20m30s</t>
+  </si>
+  <si>
+    <t>22m55s</t>
+  </si>
+  <si>
+    <t>24m43s</t>
+  </si>
+  <si>
+    <t>27m09s</t>
+  </si>
+  <si>
+    <t>29m54s</t>
+  </si>
+  <si>
+    <t>32m48s</t>
+  </si>
+  <si>
+    <t>36m48s</t>
+  </si>
+  <si>
+    <t>40m44s</t>
+  </si>
+  <si>
+    <t>44m19s</t>
+  </si>
+  <si>
+    <t>49m29s</t>
+  </si>
+  <si>
+    <t>55m38s</t>
+  </si>
+  <si>
+    <t>59m54s</t>
+  </si>
+  <si>
+    <t>13m03s</t>
+  </si>
+  <si>
+    <t>13m31s</t>
+  </si>
+  <si>
+    <t>14m31s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15m43s </t>
+  </si>
+  <si>
+    <t>17m03s</t>
+  </si>
+  <si>
+    <t>20m32s</t>
+  </si>
+  <si>
+    <t>23m15s</t>
+  </si>
+  <si>
+    <t>25m00s</t>
+  </si>
+  <si>
+    <t>27m20s</t>
+  </si>
+  <si>
+    <t>29m49s</t>
+  </si>
+  <si>
+    <t>33m07s</t>
+  </si>
+  <si>
+    <t>36m06s</t>
+  </si>
+  <si>
+    <t>40m28s</t>
+  </si>
+  <si>
+    <t>45m02s</t>
+  </si>
+  <si>
+    <t>50m50s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56m57s </t>
+  </si>
+  <si>
+    <t>13m28s</t>
+  </si>
+  <si>
+    <t>14m27s</t>
+  </si>
+  <si>
+    <t>15m59s</t>
+  </si>
+  <si>
+    <t>17m07s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22m42s </t>
+  </si>
+  <si>
+    <t>25m36s</t>
+  </si>
+  <si>
+    <t>27m38s</t>
+  </si>
+  <si>
+    <t>30m09s</t>
+  </si>
+  <si>
+    <t>33m28s</t>
+  </si>
+  <si>
+    <t>36m09s</t>
+  </si>
+  <si>
+    <t>40m30s</t>
+  </si>
+  <si>
+    <t>45m01s</t>
+  </si>
+  <si>
+    <t>51m06s</t>
+  </si>
+  <si>
+    <t>55m14s</t>
+  </si>
+  <si>
+    <t>13m05s</t>
+  </si>
+  <si>
+    <t>13m02s</t>
   </si>
 </sst>
 </file>
@@ -254,8 +500,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -295,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -313,6 +573,13 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -330,377 +597,18 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout/>
-      <c:line3DChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'1.csv'!$G$2:$G$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>100.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'1.csv'!$G$21:$G$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>250.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>243.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>230.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>222.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>212.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>203.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>192.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>181.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>180.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'1.csv'!$G$41:$G$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>434.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>400.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>371.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>348.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>328.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>312.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>293.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>281.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>266.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>243.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>230.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>222.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>212.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>203.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>192.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>181.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>180.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2132348216"/>
-        <c:axId val="2101293928"/>
-        <c:axId val="2134565400"/>
-      </c:line3DChart>
-      <c:catAx>
-        <c:axId val="2132348216"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101293928"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2101293928"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132348216"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:serAx>
-        <c:axId val="2134565400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101293928"/>
-      </c:serAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>717550</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1027,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="L129" sqref="L129"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2379,6 +2287,9 @@
       <c r="B59">
         <v>1000</v>
       </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
       <c r="D59">
         <v>7.9055329827899996</v>
       </c>
@@ -2387,6 +2298,9 @@
       </c>
       <c r="F59">
         <v>132307</v>
+      </c>
+      <c r="G59">
+        <v>434</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2396,6 +2310,9 @@
       <c r="B60">
         <v>1000</v>
       </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
       <c r="D60">
         <v>7.9055329827899996</v>
       </c>
@@ -2404,6 +2321,9 @@
       </c>
       <c r="F60">
         <v>132307</v>
+      </c>
+      <c r="G60">
+        <v>434</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2413,6 +2333,9 @@
       <c r="B61">
         <v>1000</v>
       </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
       <c r="D61">
         <v>9.5584757948599997</v>
       </c>
@@ -2421,6 +2344,9 @@
       </c>
       <c r="F61">
         <v>119653</v>
+      </c>
+      <c r="G61">
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2430,6 +2356,9 @@
       <c r="B62">
         <v>1000</v>
       </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
       <c r="D62">
         <v>11.192578044199999</v>
       </c>
@@ -2438,6 +2367,9 @@
       </c>
       <c r="F62">
         <v>108277</v>
+      </c>
+      <c r="G62">
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2447,6 +2379,9 @@
       <c r="B63">
         <v>1000</v>
       </c>
+      <c r="C63" t="s">
+        <v>71</v>
+      </c>
       <c r="D63">
         <v>12.8217783</v>
       </c>
@@ -2455,6 +2390,9 @@
       </c>
       <c r="F63">
         <v>98202</v>
+      </c>
+      <c r="G63">
+        <v>348</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2464,6 +2402,9 @@
       <c r="B64">
         <v>1000</v>
       </c>
+      <c r="C64" t="s">
+        <v>70</v>
+      </c>
       <c r="D64">
         <v>14.455737174299999</v>
       </c>
@@ -2473,14 +2414,20 @@
       <c r="F64">
         <v>89322</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>8</v>
       </c>
       <c r="B65">
         <v>1000</v>
       </c>
+      <c r="C65" t="s">
+        <v>69</v>
+      </c>
       <c r="D65">
         <v>16.086587771200001</v>
       </c>
@@ -2490,14 +2437,20 @@
       <c r="F65">
         <v>81559</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>9</v>
       </c>
       <c r="B66">
         <v>1000</v>
       </c>
+      <c r="C66" t="s">
+        <v>68</v>
+      </c>
       <c r="D66">
         <v>17.561333955199999</v>
       </c>
@@ -2507,14 +2460,20 @@
       <c r="F66">
         <v>75303</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>10</v>
       </c>
       <c r="B67">
         <v>1000</v>
       </c>
+      <c r="C67" t="s">
+        <v>67</v>
+      </c>
       <c r="D67">
         <v>19.066081710999999</v>
       </c>
@@ -2524,14 +2483,20 @@
       <c r="F67">
         <v>69534</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>11</v>
       </c>
       <c r="B68">
         <v>1000</v>
       </c>
+      <c r="C68" t="s">
+        <v>66</v>
+      </c>
       <c r="D68">
         <v>20.570332480800001</v>
       </c>
@@ -2541,14 +2506,20 @@
       <c r="F68">
         <v>64344</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>12</v>
       </c>
       <c r="B69">
         <v>1000</v>
       </c>
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
       <c r="D69">
         <v>22.0587366088</v>
       </c>
@@ -2558,14 +2529,20 @@
       <c r="F69">
         <v>59713</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>13</v>
       </c>
       <c r="B70">
         <v>1000</v>
       </c>
+      <c r="C70" t="s">
+        <v>64</v>
+      </c>
       <c r="D70">
         <v>23.479342327200001</v>
       </c>
@@ -2575,14 +2552,20 @@
       <c r="F70">
         <v>55693</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>14</v>
       </c>
       <c r="B71" s="1">
         <v>1000</v>
       </c>
+      <c r="C71" t="s">
+        <v>63</v>
+      </c>
       <c r="D71">
         <v>25.060650169799999</v>
       </c>
@@ -2592,14 +2575,20 @@
       <c r="F71">
         <v>51650</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>15</v>
       </c>
       <c r="B72" s="1">
         <v>1000</v>
       </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
       <c r="D72">
         <v>26.566703417900001</v>
       </c>
@@ -2609,14 +2598,20 @@
       <c r="F72">
         <v>48192</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>16</v>
       </c>
       <c r="B73" s="1">
         <v>1000</v>
       </c>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
       <c r="D73">
         <v>28.237854889600001</v>
       </c>
@@ -2626,14 +2621,20 @@
       <c r="F73">
         <v>44757</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>17</v>
       </c>
       <c r="B74" s="1">
         <v>1000</v>
       </c>
+      <c r="C74" t="s">
+        <v>49</v>
+      </c>
       <c r="D74">
         <v>29.756737588699998</v>
       </c>
@@ -2643,14 +2644,20 @@
       <c r="F74">
         <v>41957</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>18</v>
       </c>
       <c r="B75" s="1">
         <v>1000</v>
       </c>
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
       <c r="D75">
         <v>31.286735504399999</v>
       </c>
@@ -2660,14 +2667,20 @@
       <c r="F75">
         <v>39390</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>19</v>
       </c>
       <c r="B76" s="1">
         <v>1000</v>
       </c>
+      <c r="C76" t="s">
+        <v>60</v>
+      </c>
       <c r="D76">
         <v>32.673684210499999</v>
       </c>
@@ -2677,14 +2690,20 @@
       <c r="F76">
         <v>37248</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>20</v>
       </c>
       <c r="B77" s="1">
         <v>1000</v>
       </c>
+      <c r="C77" t="s">
+        <v>75</v>
+      </c>
       <c r="D77">
         <v>34.090029041599998</v>
       </c>
@@ -2694,14 +2713,20 @@
       <c r="F77">
         <v>35215</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>2</v>
       </c>
       <c r="B78" s="1">
         <v>2000</v>
       </c>
+      <c r="C78" t="s">
+        <v>78</v>
+      </c>
       <c r="D78">
         <v>7.9055329827899996</v>
       </c>
@@ -2711,14 +2736,20 @@
       <c r="F78">
         <v>132307</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>3</v>
       </c>
       <c r="B79" s="1">
         <v>2000</v>
       </c>
+      <c r="C79" t="s">
+        <v>78</v>
+      </c>
       <c r="D79">
         <v>7.9055329827899996</v>
       </c>
@@ -2728,14 +2759,20 @@
       <c r="F79">
         <v>132307</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>4</v>
       </c>
       <c r="B80" s="1">
         <v>2000</v>
       </c>
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
       <c r="D80">
         <v>9.5584757948599997</v>
       </c>
@@ -2745,14 +2782,20 @@
       <c r="F80">
         <v>119653</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>5</v>
       </c>
       <c r="B81" s="1">
         <v>2000</v>
       </c>
+      <c r="C81" t="s">
+        <v>91</v>
+      </c>
       <c r="D81">
         <v>11.192578044199999</v>
       </c>
@@ -2762,14 +2805,20 @@
       <c r="F81">
         <v>108277</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>6</v>
       </c>
       <c r="B82" s="1">
         <v>2000</v>
       </c>
+      <c r="C82" t="s">
+        <v>90</v>
+      </c>
       <c r="D82">
         <v>12.8217783</v>
       </c>
@@ -2779,14 +2828,20 @@
       <c r="F82">
         <v>98202</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>7</v>
       </c>
       <c r="B83" s="1">
         <v>2000</v>
       </c>
+      <c r="C83" t="s">
+        <v>89</v>
+      </c>
       <c r="D83">
         <v>14.455737174299999</v>
       </c>
@@ -2796,14 +2851,20 @@
       <c r="F83">
         <v>89322</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>8</v>
       </c>
       <c r="B84" s="1">
         <v>2000</v>
       </c>
+      <c r="C84" t="s">
+        <v>88</v>
+      </c>
       <c r="D84">
         <v>16.086587771200001</v>
       </c>
@@ -2813,14 +2874,20 @@
       <c r="F84">
         <v>81559</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>9</v>
       </c>
       <c r="B85" s="1">
         <v>2000</v>
       </c>
+      <c r="C85" t="s">
+        <v>87</v>
+      </c>
       <c r="D85">
         <v>17.561333955199999</v>
       </c>
@@ -2830,14 +2897,20 @@
       <c r="F85">
         <v>75303</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>10</v>
       </c>
       <c r="B86" s="1">
         <v>2000</v>
       </c>
+      <c r="C86" t="s">
+        <v>86</v>
+      </c>
       <c r="D86">
         <v>19.066081710999999</v>
       </c>
@@ -2847,14 +2920,20 @@
       <c r="F86">
         <v>69534</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>11</v>
       </c>
       <c r="B87" s="1">
         <v>2000</v>
       </c>
+      <c r="C87" t="s">
+        <v>85</v>
+      </c>
       <c r="D87">
         <v>20.570332480800001</v>
       </c>
@@ -2864,14 +2943,20 @@
       <c r="F87">
         <v>64344</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>12</v>
       </c>
       <c r="B88" s="1">
         <v>2000</v>
       </c>
+      <c r="C88" t="s">
+        <v>84</v>
+      </c>
       <c r="D88">
         <v>22.0587366088</v>
       </c>
@@ -2881,14 +2966,20 @@
       <c r="F88">
         <v>59713</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>13</v>
       </c>
       <c r="B89" s="1">
         <v>2000</v>
       </c>
+      <c r="C89" t="s">
+        <v>83</v>
+      </c>
       <c r="D89">
         <v>23.479342327200001</v>
       </c>
@@ -2898,14 +2989,20 @@
       <c r="F89">
         <v>55693</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>14</v>
       </c>
       <c r="B90" s="1">
         <v>2000</v>
       </c>
+      <c r="C90" t="s">
+        <v>82</v>
+      </c>
       <c r="D90">
         <v>25.060650169799999</v>
       </c>
@@ -2915,14 +3012,20 @@
       <c r="F90">
         <v>51650</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>15</v>
       </c>
       <c r="B91" s="1">
         <v>2000</v>
       </c>
+      <c r="C91" t="s">
+        <v>81</v>
+      </c>
       <c r="D91">
         <v>26.566703417900001</v>
       </c>
@@ -2932,14 +3035,20 @@
       <c r="F91">
         <v>48192</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>16</v>
       </c>
       <c r="B92" s="1">
         <v>2000</v>
       </c>
+      <c r="C92" t="s">
+        <v>80</v>
+      </c>
       <c r="D92">
         <v>28.237854889600001</v>
       </c>
@@ -2949,14 +3058,20 @@
       <c r="F92">
         <v>44757</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>17</v>
       </c>
       <c r="B93" s="1">
         <v>2000</v>
       </c>
+      <c r="C93" t="s">
+        <v>79</v>
+      </c>
       <c r="D93">
         <v>29.756737588699998</v>
       </c>
@@ -2966,14 +3081,20 @@
       <c r="F93">
         <v>41957</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>18</v>
       </c>
       <c r="B94" s="1">
         <v>2000</v>
       </c>
+      <c r="C94" t="s">
+        <v>77</v>
+      </c>
       <c r="D94">
         <v>31.286735504399999</v>
       </c>
@@ -2983,14 +3104,20 @@
       <c r="F94">
         <v>39390</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>19</v>
       </c>
       <c r="B95" s="1">
         <v>2000</v>
       </c>
+      <c r="C95" t="s">
+        <v>76</v>
+      </c>
       <c r="D95">
         <v>32.673684210499999</v>
       </c>
@@ -3000,14 +3127,20 @@
       <c r="F95">
         <v>37248</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>20</v>
       </c>
       <c r="B96" s="1">
         <v>2000</v>
       </c>
+      <c r="C96" t="s">
+        <v>93</v>
+      </c>
       <c r="D96">
         <v>34.090029041599998</v>
       </c>
@@ -3017,14 +3150,20 @@
       <c r="F96">
         <v>35215</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>2</v>
       </c>
       <c r="B97" s="1">
         <v>5000</v>
       </c>
+      <c r="C97" t="s">
+        <v>78</v>
+      </c>
       <c r="D97">
         <v>7.9055329827899996</v>
       </c>
@@ -3034,14 +3173,20 @@
       <c r="F97">
         <v>132307</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>3</v>
       </c>
       <c r="B98" s="1">
         <v>5000</v>
       </c>
+      <c r="C98" t="s">
+        <v>109</v>
+      </c>
       <c r="D98">
         <v>7.9055329827899996</v>
       </c>
@@ -3051,14 +3196,20 @@
       <c r="F98">
         <v>132307</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>4</v>
       </c>
       <c r="B99" s="1">
         <v>5000</v>
       </c>
+      <c r="C99" t="s">
+        <v>108</v>
+      </c>
       <c r="D99">
         <v>9.5584757948599997</v>
       </c>
@@ -3068,14 +3219,20 @@
       <c r="F99">
         <v>119653</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>5</v>
       </c>
       <c r="B100" s="1">
         <v>5000</v>
       </c>
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
       <c r="D100">
         <v>11.192578044199999</v>
       </c>
@@ -3085,14 +3242,20 @@
       <c r="F100">
         <v>108277</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>6</v>
       </c>
       <c r="B101" s="1">
         <v>5000</v>
       </c>
+      <c r="C101" t="s">
+        <v>106</v>
+      </c>
       <c r="D101">
         <v>12.8217783</v>
       </c>
@@ -3102,14 +3265,20 @@
       <c r="F101">
         <v>98202</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>7</v>
       </c>
       <c r="B102" s="1">
         <v>5000</v>
       </c>
+      <c r="C102" t="s">
+        <v>105</v>
+      </c>
       <c r="D102">
         <v>14.455737174299999</v>
       </c>
@@ -3119,14 +3288,20 @@
       <c r="F102">
         <v>89322</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>8</v>
       </c>
       <c r="B103" s="1">
         <v>5000</v>
       </c>
+      <c r="C103" t="s">
+        <v>104</v>
+      </c>
       <c r="D103">
         <v>16.086587771200001</v>
       </c>
@@ -3136,14 +3311,20 @@
       <c r="F103">
         <v>81559</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>9</v>
       </c>
       <c r="B104" s="1">
         <v>5000</v>
       </c>
+      <c r="C104" t="s">
+        <v>103</v>
+      </c>
       <c r="D104">
         <v>17.561333955199999</v>
       </c>
@@ -3153,14 +3334,20 @@
       <c r="F104">
         <v>75303</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>10</v>
       </c>
       <c r="B105" s="1">
         <v>5000</v>
       </c>
+      <c r="C105" t="s">
+        <v>102</v>
+      </c>
       <c r="D105">
         <v>19.066081710999999</v>
       </c>
@@ -3170,14 +3357,20 @@
       <c r="F105">
         <v>69534</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>11</v>
       </c>
       <c r="B106" s="1">
         <v>5000</v>
       </c>
+      <c r="C106" t="s">
+        <v>101</v>
+      </c>
       <c r="D106">
         <v>20.570332480800001</v>
       </c>
@@ -3187,14 +3380,20 @@
       <c r="F106">
         <v>64344</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>12</v>
       </c>
       <c r="B107" s="1">
         <v>5000</v>
       </c>
+      <c r="C107" t="s">
+        <v>100</v>
+      </c>
       <c r="D107">
         <v>22.0587366088</v>
       </c>
@@ -3204,14 +3403,20 @@
       <c r="F107">
         <v>59713</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="G107">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>13</v>
       </c>
       <c r="B108" s="1">
         <v>5000</v>
       </c>
+      <c r="C108" t="s">
+        <v>99</v>
+      </c>
       <c r="D108">
         <v>23.479342327200001</v>
       </c>
@@ -3221,14 +3426,20 @@
       <c r="F108">
         <v>55693</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="G108">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>14</v>
       </c>
       <c r="B109" s="1">
         <v>5000</v>
       </c>
+      <c r="C109" t="s">
+        <v>98</v>
+      </c>
       <c r="D109">
         <v>25.060650169799999</v>
       </c>
@@ -3238,14 +3449,20 @@
       <c r="F109">
         <v>51650</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="G109">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>15</v>
       </c>
       <c r="B110" s="1">
         <v>5000</v>
       </c>
+      <c r="C110" t="s">
+        <v>97</v>
+      </c>
       <c r="D110">
         <v>26.566703417900001</v>
       </c>
@@ -3255,14 +3472,20 @@
       <c r="F110">
         <v>48192</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>16</v>
       </c>
       <c r="B111" s="1">
         <v>5000</v>
       </c>
+      <c r="C111" t="s">
+        <v>96</v>
+      </c>
       <c r="D111">
         <v>28.237854889600001</v>
       </c>
@@ -3272,14 +3495,20 @@
       <c r="F111">
         <v>44757</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>17</v>
       </c>
       <c r="B112" s="1">
         <v>5000</v>
       </c>
+      <c r="C112" t="s">
+        <v>14</v>
+      </c>
       <c r="D112">
         <v>29.756737588699998</v>
       </c>
@@ -3289,14 +3518,20 @@
       <c r="F112">
         <v>41957</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>18</v>
       </c>
       <c r="B113" s="1">
         <v>5000</v>
       </c>
+      <c r="C113" t="s">
+        <v>95</v>
+      </c>
       <c r="D113">
         <v>31.286735504399999</v>
       </c>
@@ -3306,14 +3541,20 @@
       <c r="F113">
         <v>39390</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>19</v>
       </c>
       <c r="B114" s="1">
         <v>5000</v>
       </c>
+      <c r="C114" t="s">
+        <v>94</v>
+      </c>
       <c r="D114">
         <v>32.673684210499999</v>
       </c>
@@ -3323,14 +3564,20 @@
       <c r="F114">
         <v>37248</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>20</v>
       </c>
       <c r="B115" s="1">
         <v>5000</v>
       </c>
+      <c r="C115" t="s">
+        <v>110</v>
+      </c>
       <c r="D115">
         <v>34.090029041599998</v>
       </c>
@@ -3340,14 +3587,20 @@
       <c r="F115">
         <v>35215</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>2</v>
       </c>
       <c r="B116" s="1">
         <v>10000</v>
       </c>
+      <c r="C116" t="s">
+        <v>19</v>
+      </c>
       <c r="D116">
         <v>7.9055329827899996</v>
       </c>
@@ -3357,14 +3610,20 @@
       <c r="F116">
         <v>132307</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117">
         <v>3</v>
       </c>
       <c r="B117" s="1">
         <v>10000</v>
       </c>
+      <c r="C117" t="s">
+        <v>19</v>
+      </c>
       <c r="D117">
         <v>7.9055329827899996</v>
       </c>
@@ -3374,14 +3633,20 @@
       <c r="F117">
         <v>132307</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118">
         <v>4</v>
       </c>
       <c r="B118" s="1">
         <v>10000</v>
       </c>
+      <c r="C118" t="s">
+        <v>125</v>
+      </c>
       <c r="D118">
         <v>9.5584757948599997</v>
       </c>
@@ -3391,14 +3656,20 @@
       <c r="F118">
         <v>119653</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119">
         <v>5</v>
       </c>
       <c r="B119" s="1">
         <v>10000</v>
       </c>
+      <c r="C119" t="s">
+        <v>124</v>
+      </c>
       <c r="D119">
         <v>11.192578044199999</v>
       </c>
@@ -3408,14 +3679,20 @@
       <c r="F119">
         <v>108277</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119" s="1">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120">
         <v>6</v>
       </c>
       <c r="B120" s="1">
         <v>10000</v>
       </c>
+      <c r="C120" t="s">
+        <v>123</v>
+      </c>
       <c r="D120">
         <v>12.8217783</v>
       </c>
@@ -3425,14 +3702,20 @@
       <c r="F120">
         <v>98202</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120" s="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121">
         <v>7</v>
       </c>
       <c r="B121" s="1">
         <v>10000</v>
       </c>
+      <c r="C121" t="s">
+        <v>122</v>
+      </c>
       <c r="D121">
         <v>14.455737174299999</v>
       </c>
@@ -3442,14 +3725,20 @@
       <c r="F121">
         <v>89322</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121" s="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122">
         <v>8</v>
       </c>
       <c r="B122" s="1">
         <v>10000</v>
       </c>
+      <c r="C122" t="s">
+        <v>121</v>
+      </c>
       <c r="D122">
         <v>16.086587771200001</v>
       </c>
@@ -3459,14 +3748,20 @@
       <c r="F122">
         <v>81559</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122" s="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123">
         <v>9</v>
       </c>
       <c r="B123" s="1">
         <v>10000</v>
       </c>
+      <c r="C123" t="s">
+        <v>120</v>
+      </c>
       <c r="D123">
         <v>17.561333955199999</v>
       </c>
@@ -3476,14 +3771,20 @@
       <c r="F123">
         <v>75303</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="G123" s="1">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
       <c r="A124">
         <v>10</v>
       </c>
       <c r="B124" s="1">
         <v>10000</v>
       </c>
+      <c r="C124" t="s">
+        <v>119</v>
+      </c>
       <c r="D124">
         <v>19.066081710999999</v>
       </c>
@@ -3493,14 +3794,20 @@
       <c r="F124">
         <v>69534</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="G124" s="1">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125">
         <v>11</v>
       </c>
       <c r="B125" s="1">
         <v>10000</v>
       </c>
+      <c r="C125" t="s">
+        <v>118</v>
+      </c>
       <c r="D125">
         <v>20.570332480800001</v>
       </c>
@@ -3510,14 +3817,20 @@
       <c r="F125">
         <v>64344</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125" s="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126">
         <v>12</v>
       </c>
       <c r="B126" s="1">
         <v>10000</v>
       </c>
+      <c r="C126" t="s">
+        <v>117</v>
+      </c>
       <c r="D126">
         <v>22.0587366088</v>
       </c>
@@ -3527,14 +3840,20 @@
       <c r="F126">
         <v>59713</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126" s="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127">
         <v>13</v>
       </c>
       <c r="B127" s="1">
         <v>10000</v>
       </c>
+      <c r="C127" t="s">
+        <v>116</v>
+      </c>
       <c r="D127">
         <v>23.479342327200001</v>
       </c>
@@ -3544,14 +3863,20 @@
       <c r="F127">
         <v>55693</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="G127" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128">
         <v>14</v>
       </c>
       <c r="B128" s="1">
         <v>10000</v>
       </c>
+      <c r="C128" t="s">
+        <v>115</v>
+      </c>
       <c r="D128">
         <v>25.060650169799999</v>
       </c>
@@ -3561,14 +3886,20 @@
       <c r="F128">
         <v>51650</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="G128" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
       <c r="A129">
         <v>15</v>
       </c>
       <c r="B129" s="1">
         <v>10000</v>
       </c>
+      <c r="C129" t="s">
+        <v>81</v>
+      </c>
       <c r="D129">
         <v>26.566703417900001</v>
       </c>
@@ -3578,14 +3909,20 @@
       <c r="F129">
         <v>48192</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129" s="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
       <c r="A130">
         <v>16</v>
       </c>
       <c r="B130" s="1">
         <v>10000</v>
       </c>
+      <c r="C130" t="s">
+        <v>114</v>
+      </c>
       <c r="D130">
         <v>28.237854889600001</v>
       </c>
@@ -3595,14 +3932,20 @@
       <c r="F130">
         <v>44757</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130" s="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
       <c r="A131">
         <v>17</v>
       </c>
       <c r="B131" s="1">
         <v>10000</v>
       </c>
+      <c r="C131" t="s">
+        <v>113</v>
+      </c>
       <c r="D131">
         <v>29.756737588699998</v>
       </c>
@@ -3612,14 +3955,20 @@
       <c r="F131">
         <v>41957</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="G131" s="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
       <c r="A132">
         <v>18</v>
       </c>
       <c r="B132" s="1">
         <v>10000</v>
       </c>
+      <c r="C132" t="s">
+        <v>112</v>
+      </c>
       <c r="D132">
         <v>31.286735504399999</v>
       </c>
@@ -3629,14 +3978,20 @@
       <c r="F132">
         <v>39390</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
       <c r="A133">
         <v>19</v>
       </c>
       <c r="B133" s="1">
         <v>10000</v>
       </c>
+      <c r="C133" t="s">
+        <v>111</v>
+      </c>
       <c r="D133">
         <v>32.673684210499999</v>
       </c>
@@ -3646,14 +4001,20 @@
       <c r="F133">
         <v>37248</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133" s="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
       <c r="A134">
         <v>20</v>
       </c>
       <c r="B134" s="1">
         <v>10000</v>
       </c>
+      <c r="C134" t="s">
+        <v>140</v>
+      </c>
       <c r="D134">
         <v>34.090029041599998</v>
       </c>
@@ -3663,14 +4024,20 @@
       <c r="F134">
         <v>35215</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135">
         <v>2</v>
       </c>
       <c r="B135" s="1">
         <v>50000</v>
       </c>
+      <c r="C135" t="s">
+        <v>19</v>
+      </c>
       <c r="D135">
         <v>7.9055329827899996</v>
       </c>
@@ -3680,14 +4047,20 @@
       <c r="F135">
         <v>132307</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="G135" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
       <c r="A136">
         <v>3</v>
       </c>
       <c r="B136" s="1">
         <v>50000</v>
       </c>
+      <c r="C136" t="s">
+        <v>19</v>
+      </c>
       <c r="D136">
         <v>7.9055329827899996</v>
       </c>
@@ -3697,14 +4070,20 @@
       <c r="F136">
         <v>132307</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="G136" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
       <c r="A137">
         <v>4</v>
       </c>
       <c r="B137" s="1">
         <v>50000</v>
       </c>
+      <c r="C137" t="s">
+        <v>139</v>
+      </c>
       <c r="D137">
         <v>9.5584757948599997</v>
       </c>
@@ -3714,14 +4093,20 @@
       <c r="F137">
         <v>119653</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="G137" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
       <c r="A138">
         <v>5</v>
       </c>
       <c r="B138" s="1">
         <v>50000</v>
       </c>
+      <c r="C138" t="s">
+        <v>138</v>
+      </c>
       <c r="D138">
         <v>11.192578044199999</v>
       </c>
@@ -3731,14 +4116,20 @@
       <c r="F138">
         <v>108277</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="G138" s="1">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
       <c r="A139">
         <v>6</v>
       </c>
       <c r="B139" s="1">
         <v>50000</v>
       </c>
+      <c r="C139" t="s">
+        <v>137</v>
+      </c>
       <c r="D139">
         <v>12.8217783</v>
       </c>
@@ -3748,14 +4139,20 @@
       <c r="F139">
         <v>98202</v>
       </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="G139" s="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
       <c r="A140">
         <v>7</v>
       </c>
       <c r="B140" s="1">
         <v>50000</v>
       </c>
+      <c r="C140" t="s">
+        <v>136</v>
+      </c>
       <c r="D140">
         <v>14.455737174299999</v>
       </c>
@@ -3765,14 +4162,20 @@
       <c r="F140">
         <v>89322</v>
       </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="G140" s="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
       <c r="A141">
         <v>8</v>
       </c>
       <c r="B141" s="1">
         <v>50000</v>
       </c>
+      <c r="C141" t="s">
+        <v>135</v>
+      </c>
       <c r="D141">
         <v>16.086587771200001</v>
       </c>
@@ -3782,14 +4185,20 @@
       <c r="F141">
         <v>81559</v>
       </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="G141" s="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
       <c r="A142">
         <v>9</v>
       </c>
       <c r="B142" s="1">
         <v>50000</v>
       </c>
+      <c r="C142" t="s">
+        <v>134</v>
+      </c>
       <c r="D142">
         <v>17.561333955199999</v>
       </c>
@@ -3799,14 +4208,20 @@
       <c r="F142">
         <v>75303</v>
       </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="G142" s="1">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
       <c r="A143">
         <v>10</v>
       </c>
       <c r="B143" s="1">
         <v>50000</v>
       </c>
+      <c r="C143" t="s">
+        <v>133</v>
+      </c>
       <c r="D143">
         <v>19.066081710999999</v>
       </c>
@@ -3816,14 +4231,20 @@
       <c r="F143">
         <v>69534</v>
       </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="G143" s="1">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
       <c r="A144">
         <v>11</v>
       </c>
       <c r="B144" s="1">
         <v>50000</v>
       </c>
+      <c r="C144" t="s">
+        <v>132</v>
+      </c>
       <c r="D144">
         <v>20.570332480800001</v>
       </c>
@@ -3833,14 +4254,20 @@
       <c r="F144">
         <v>64344</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="G144" s="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
       <c r="A145">
         <v>12</v>
       </c>
       <c r="B145" s="1">
         <v>50000</v>
       </c>
+      <c r="C145" t="s">
+        <v>131</v>
+      </c>
       <c r="D145">
         <v>22.0587366088</v>
       </c>
@@ -3850,14 +4277,20 @@
       <c r="F145">
         <v>59713</v>
       </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="G145" s="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
       <c r="A146">
         <v>13</v>
       </c>
       <c r="B146" s="1">
         <v>50000</v>
       </c>
+      <c r="C146" t="s">
+        <v>130</v>
+      </c>
       <c r="D146">
         <v>23.479342327200001</v>
       </c>
@@ -3867,14 +4300,20 @@
       <c r="F146">
         <v>55693</v>
       </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="G146" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
       <c r="A147">
         <v>14</v>
       </c>
       <c r="B147" s="1">
         <v>50000</v>
       </c>
+      <c r="C147" t="s">
+        <v>46</v>
+      </c>
       <c r="D147">
         <v>25.060650169799999</v>
       </c>
@@ -3884,14 +4323,20 @@
       <c r="F147">
         <v>51650</v>
       </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="G147" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
       <c r="A148">
         <v>15</v>
       </c>
       <c r="B148" s="1">
         <v>50000</v>
       </c>
+      <c r="C148" t="s">
+        <v>47</v>
+      </c>
       <c r="D148">
         <v>26.566703417900001</v>
       </c>
@@ -3901,14 +4346,20 @@
       <c r="F148">
         <v>48192</v>
       </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="G148" s="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
       <c r="A149">
         <v>16</v>
       </c>
       <c r="B149" s="1">
         <v>50000</v>
       </c>
+      <c r="C149" t="s">
+        <v>129</v>
+      </c>
       <c r="D149">
         <v>28.237854889600001</v>
       </c>
@@ -3918,14 +4369,20 @@
       <c r="F149">
         <v>44757</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="G149" s="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
       <c r="A150">
         <v>17</v>
       </c>
       <c r="B150" s="1">
         <v>50000</v>
       </c>
+      <c r="C150" t="s">
+        <v>128</v>
+      </c>
       <c r="D150">
         <v>29.756737588699998</v>
       </c>
@@ -3935,14 +4392,20 @@
       <c r="F150">
         <v>41957</v>
       </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="G150" s="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
       <c r="A151">
         <v>18</v>
       </c>
       <c r="B151" s="1">
         <v>50000</v>
       </c>
+      <c r="C151" t="s">
+        <v>127</v>
+      </c>
       <c r="D151">
         <v>31.286735504399999</v>
       </c>
@@ -3952,14 +4415,20 @@
       <c r="F151">
         <v>39390</v>
       </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="G151" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
       <c r="A152">
         <v>19</v>
       </c>
       <c r="B152" s="1">
         <v>50000</v>
       </c>
+      <c r="C152" t="s">
+        <v>126</v>
+      </c>
       <c r="D152">
         <v>32.673684210499999</v>
       </c>
@@ -3969,14 +4438,20 @@
       <c r="F152">
         <v>37248</v>
       </c>
-    </row>
-    <row r="153" spans="1:6">
+      <c r="G152" s="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
       <c r="A153">
         <v>20</v>
       </c>
       <c r="B153" s="1">
         <v>50000</v>
       </c>
+      <c r="C153" t="s">
+        <v>141</v>
+      </c>
       <c r="D153">
         <v>34.090029041599998</v>
       </c>
@@ -3985,12 +4460,14 @@
       </c>
       <c r="F153">
         <v>35215</v>
+      </c>
+      <c r="G153" s="1">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>